<commit_message>
Employee Creation script completed
</commit_message>
<xml_diff>
--- a/Data/ConfigData/EmployeeCreationConfig.xlsx
+++ b/Data/ConfigData/EmployeeCreationConfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>TestId</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>ResEmployeeCreation</t>
+  </si>
+  <si>
+    <t>newemp_002</t>
+  </si>
+  <si>
+    <t>newemp_003</t>
   </si>
 </sst>
 </file>
@@ -99,10 +105,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -115,13 +121,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -136,6 +135,97 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -152,21 +242,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -174,45 +264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -222,51 +273,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,37 +287,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,145 +461,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,6 +486,36 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,36 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -575,148 +581,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1043,13 +1049,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="24.5714285714286" customWidth="1"/>
@@ -1188,9 +1194,119 @@
         <v>1</v>
       </c>
       <c r="T2" s="2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="U2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>4</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <v>55</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="2">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>4</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>55</v>
+      </c>
+      <c r="U4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>